<commit_message>
disabled csrf, login and register works
</commit_message>
<xml_diff>
--- a/Database Grading Criteria (2).xlsx
+++ b/Database Grading Criteria (2).xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="51">
   <si>
     <t xml:space="preserve">Grading Element</t>
   </si>
@@ -56,6 +56,9 @@
   </si>
   <si>
     <t xml:space="preserve">ALTER TABLE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">arguable</t>
   </si>
   <si>
     <t xml:space="preserve">DROP obj</t>
@@ -294,32 +297,36 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -575,468 +582,439 @@
   <dimension ref="A1:C48"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C45" activeCellId="0" sqref="C45"/>
+      <selection pane="topLeft" activeCell="C17" activeCellId="0" sqref="C17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.57421875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="26.73"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="5.91"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="29.04"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="5.91"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="3" t="n">
+      <c r="A2" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="4" t="n">
         <v>5</v>
       </c>
-      <c r="C2" s="0" t="s">
+      <c r="C2" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="3" t="n">
+      <c r="B3" s="4" t="n">
         <v>5</v>
       </c>
-      <c r="C3" s="0" t="s">
+      <c r="C3" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="3" t="n">
+      <c r="B4" s="4" t="n">
         <v>5</v>
       </c>
-      <c r="C4" s="0" t="s">
+      <c r="C4" s="1"/>
+    </row>
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="4" t="n">
+        <v>5</v>
+      </c>
+      <c r="C5" s="1"/>
+    </row>
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="4" t="n">
+        <v>5</v>
+      </c>
+      <c r="C6" s="1"/>
+    </row>
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" s="4" t="n">
+        <v>5</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" s="3" t="n">
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" s="4" t="n">
         <v>5</v>
       </c>
-      <c r="C5" s="0" t="s">
+    </row>
+    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" s="4" t="n">
         <v>3</v>
       </c>
-    </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B6" s="3" t="n">
-        <v>5</v>
-      </c>
-      <c r="C6" s="0" t="s">
+      <c r="C9" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B7" s="3" t="n">
-        <v>5</v>
-      </c>
-      <c r="C7" s="0" t="s">
+    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" s="4" t="n">
+        <v>2</v>
+      </c>
+      <c r="C10" s="0" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11" s="4" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B12" s="4" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B13" s="4" t="n">
+        <v>2</v>
+      </c>
+      <c r="C13" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B8" s="3" t="n">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B9" s="3" t="n">
+    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B14" s="4" t="n">
+        <v>2</v>
+      </c>
+      <c r="C14" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C9" s="0" t="s">
+    </row>
+    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B15" s="4" t="n">
+        <v>2</v>
+      </c>
+      <c r="C15" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B10" s="3" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="B11" s="3" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B12" s="3" t="n">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="B13" s="3" t="n">
-        <v>2</v>
-      </c>
-      <c r="C13" s="0" t="s">
+    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B16" s="4" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B17" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="C17" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="B14" s="3" t="n">
-        <v>2</v>
-      </c>
-      <c r="C14" s="0" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="B15" s="3" t="n">
-        <v>2</v>
-      </c>
-      <c r="C15" s="0" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="B16" s="3" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="B17" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="C17" s="0" t="s">
-        <v>3</v>
-      </c>
-    </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="B18" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="C18" s="0" t="s">
-        <v>3</v>
-      </c>
+      <c r="A18" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B18" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="C18" s="1"/>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="B19" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="C19" s="0" t="s">
-        <v>3</v>
-      </c>
+      <c r="A19" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B19" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="C19" s="1"/>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="B20" s="3" t="n">
-        <v>2</v>
-      </c>
-      <c r="C20" s="0" t="s">
-        <v>3</v>
-      </c>
+      <c r="A20" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B20" s="4" t="n">
+        <v>2</v>
+      </c>
+      <c r="C20" s="1"/>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="B21" s="3" t="n">
-        <v>2</v>
-      </c>
-      <c r="C21" s="0" t="s">
-        <v>3</v>
-      </c>
+      <c r="A21" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B21" s="4" t="n">
+        <v>2</v>
+      </c>
+      <c r="C21" s="1"/>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="B22" s="3" t="n">
+      <c r="A22" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B22" s="4" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="B23" s="3" t="n">
-        <v>2</v>
-      </c>
-      <c r="C23" s="0" t="s">
-        <v>3</v>
-      </c>
+      <c r="A23" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="B23" s="4" t="n">
+        <v>2</v>
+      </c>
+      <c r="C23" s="1"/>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="B24" s="3" t="n">
-        <v>2</v>
-      </c>
-      <c r="C24" s="0" t="s">
-        <v>3</v>
-      </c>
+      <c r="A24" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="B24" s="4" t="n">
+        <v>2</v>
+      </c>
+      <c r="C24" s="1"/>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="B25" s="3" t="n">
+      <c r="A25" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="B25" s="4" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="B26" s="3" t="n">
+      <c r="A26" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="B26" s="4" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="B27" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="C27" s="0" t="s">
-        <v>3</v>
-      </c>
+      <c r="A27" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="B27" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="C27" s="1"/>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="B28" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="C28" s="0" t="s">
-        <v>3</v>
-      </c>
+      <c r="A28" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="B28" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="C28" s="1"/>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="B29" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="C29" s="0" t="s">
-        <v>3</v>
-      </c>
+      <c r="A29" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="B29" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="C29" s="1"/>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="B30" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="C30" s="0" t="s">
-        <v>3</v>
-      </c>
+      <c r="A30" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="B30" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="C30" s="1"/>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="B31" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="C31" s="0" t="s">
-        <v>3</v>
-      </c>
+      <c r="A31" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="B31" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="C31" s="1"/>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="B32" s="3" t="n">
+      <c r="A32" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="B32" s="4" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="B33" s="3" t="n">
+      <c r="A33" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="B33" s="4" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="B34" s="3" t="n">
+      <c r="A34" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="B34" s="4" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="B35" s="3" t="n">
+      <c r="A35" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="B35" s="4" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="B36" s="3" t="n">
+      <c r="A36" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="B36" s="4" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="B37" s="3" t="n">
+      <c r="A37" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="B37" s="4" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="B38" s="3" t="n">
+      <c r="A38" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="B38" s="4" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="B39" s="3" t="n">
+      <c r="A39" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="B39" s="4" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="B40" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="C40" s="0" t="s">
-        <v>3</v>
-      </c>
+      <c r="A40" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="B40" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="C40" s="1"/>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="B41" s="3" t="n">
+      <c r="A41" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="B41" s="4" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="B42" s="3" t="n">
+      <c r="A42" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="B42" s="4" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="B43" s="3" t="n">
+      <c r="A43" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="B43" s="4" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="B44" s="3" t="n">
-        <v>2</v>
-      </c>
-      <c r="C44" s="0" t="s">
-        <v>3</v>
-      </c>
+      <c r="A44" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="B44" s="4" t="n">
+        <v>2</v>
+      </c>
+      <c r="C44" s="1"/>
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="B45" s="3" t="n">
+      <c r="A45" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="B45" s="4" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="B46" s="3" t="n">
+      <c r="A46" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="B46" s="4" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="B47" s="3" t="n">
+      <c r="A47" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="B47" s="4" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="B48" s="1" t="n">
+      <c r="A48" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="B48" s="2" t="n">
         <f aca="false">SUM(B2:B47)</f>
         <v>100</v>
       </c>

</xml_diff>

<commit_message>
updated comments and criteria
</commit_message>
<xml_diff>
--- a/Database Grading Criteria (2).xlsx
+++ b/Database Grading Criteria (2).xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="50">
   <si>
     <t xml:space="preserve">Grading Element</t>
   </si>
@@ -56,9 +56,6 @@
   </si>
   <si>
     <t xml:space="preserve">ALTER TABLE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">arguable</t>
   </si>
   <si>
     <t xml:space="preserve">DROP obj</t>
@@ -582,7 +579,7 @@
   <dimension ref="A1:C48"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C17" activeCellId="0" sqref="C17"/>
+      <selection pane="topLeft" activeCell="C29" activeCellId="0" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.57421875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -637,7 +634,9 @@
       <c r="B5" s="4" t="n">
         <v>5</v>
       </c>
-      <c r="C5" s="1"/>
+      <c r="C5" s="1" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="s">
@@ -666,6 +665,9 @@
       <c r="B8" s="4" t="n">
         <v>5</v>
       </c>
+      <c r="C8" s="0" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="5" t="s">
@@ -685,13 +687,13 @@
       <c r="B10" s="4" t="n">
         <v>2</v>
       </c>
-      <c r="C10" s="0" t="s">
-        <v>12</v>
+      <c r="C10" s="1" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B11" s="4" t="n">
         <v>2</v>
@@ -699,7 +701,7 @@
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B12" s="4" t="n">
         <v>4</v>
@@ -707,7 +709,7 @@
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B13" s="4" t="n">
         <v>2</v>
@@ -718,7 +720,7 @@
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B14" s="4" t="n">
         <v>2</v>
@@ -729,26 +731,27 @@
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B15" s="4" t="n">
         <v>2</v>
       </c>
-      <c r="C15" s="1" t="s">
-        <v>3</v>
-      </c>
+      <c r="C15" s="1"/>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B16" s="4" t="n">
         <v>2</v>
+      </c>
+      <c r="C16" s="0" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B17" s="4" t="n">
         <v>1</v>
@@ -759,7 +762,7 @@
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B18" s="4" t="n">
         <v>1</v>
@@ -768,7 +771,7 @@
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B19" s="4" t="n">
         <v>1</v>
@@ -777,7 +780,7 @@
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B20" s="4" t="n">
         <v>2</v>
@@ -786,7 +789,7 @@
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B21" s="4" t="n">
         <v>2</v>
@@ -795,7 +798,7 @@
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B22" s="4" t="n">
         <v>2</v>
@@ -803,7 +806,7 @@
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B23" s="4" t="n">
         <v>2</v>
@@ -812,7 +815,7 @@
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B24" s="4" t="n">
         <v>2</v>
@@ -821,23 +824,29 @@
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B25" s="4" t="n">
         <v>1</v>
+      </c>
+      <c r="C25" s="0" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B26" s="4" t="n">
         <v>1</v>
+      </c>
+      <c r="C26" s="0" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B27" s="4" t="n">
         <v>1</v>
@@ -846,7 +855,7 @@
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B28" s="4" t="n">
         <v>1</v>
@@ -855,7 +864,7 @@
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B29" s="4" t="n">
         <v>1</v>
@@ -864,7 +873,7 @@
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B30" s="4" t="n">
         <v>1</v>
@@ -873,7 +882,7 @@
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B31" s="4" t="n">
         <v>1</v>
@@ -882,7 +891,7 @@
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B32" s="4" t="n">
         <v>2</v>
@@ -890,7 +899,7 @@
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B33" s="4" t="n">
         <v>2</v>
@@ -898,7 +907,7 @@
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B34" s="4" t="n">
         <v>2</v>
@@ -906,7 +915,7 @@
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B35" s="4" t="n">
         <v>1</v>
@@ -914,7 +923,7 @@
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B36" s="4" t="n">
         <v>1</v>
@@ -922,7 +931,7 @@
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B37" s="4" t="n">
         <v>1</v>
@@ -930,7 +939,7 @@
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B38" s="4" t="n">
         <v>1</v>
@@ -938,7 +947,7 @@
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B39" s="4" t="n">
         <v>1</v>
@@ -946,7 +955,7 @@
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B40" s="4" t="n">
         <v>1</v>
@@ -955,7 +964,7 @@
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B41" s="4" t="n">
         <v>2</v>
@@ -963,7 +972,7 @@
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B42" s="4" t="n">
         <v>2</v>
@@ -971,7 +980,7 @@
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B43" s="4" t="n">
         <v>2</v>
@@ -979,7 +988,7 @@
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B44" s="4" t="n">
         <v>2</v>
@@ -988,7 +997,7 @@
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B45" s="4" t="n">
         <v>2</v>
@@ -996,7 +1005,7 @@
     </row>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B46" s="4" t="n">
         <v>2</v>
@@ -1004,7 +1013,7 @@
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B47" s="4" t="n">
         <v>2</v>
@@ -1012,7 +1021,7 @@
     </row>
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="7" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B48" s="2" t="n">
         <f aca="false">SUM(B2:B47)</f>

</xml_diff>

<commit_message>
add collection view functionality for the user and database drop function
</commit_message>
<xml_diff>
--- a/Database Grading Criteria (2).xlsx
+++ b/Database Grading Criteria (2).xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="50">
   <si>
     <t xml:space="preserve">Grading Element</t>
   </si>
@@ -579,7 +579,7 @@
   <dimension ref="A1:C48"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I26" activeCellId="0" sqref="I26"/>
+      <selection pane="topLeft" activeCell="C33" activeCellId="0" sqref="C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.57421875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -647,7 +647,9 @@
       <c r="B6" s="4" t="n">
         <v>5</v>
       </c>
-      <c r="C6" s="1"/>
+      <c r="C6" s="1" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="3" t="s">
@@ -700,6 +702,9 @@
       <c r="B11" s="4" t="n">
         <v>2</v>
       </c>
+      <c r="C11" s="0" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="5" t="s">
@@ -708,6 +713,9 @@
       <c r="B12" s="4" t="n">
         <v>4</v>
       </c>
+      <c r="C12" s="0" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="5" t="s">
@@ -738,7 +746,9 @@
       <c r="B15" s="4" t="n">
         <v>2</v>
       </c>
-      <c r="C15" s="1"/>
+      <c r="C15" s="1" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="5" t="s">
@@ -800,7 +810,9 @@
       <c r="B21" s="4" t="n">
         <v>2</v>
       </c>
-      <c r="C21" s="1"/>
+      <c r="C21" s="1" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="5" t="s">
@@ -809,6 +821,9 @@
       <c r="B22" s="4" t="n">
         <v>2</v>
       </c>
+      <c r="C22" s="0" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="6" t="s">
@@ -901,6 +916,9 @@
       </c>
       <c r="B32" s="4" t="n">
         <v>2</v>
+      </c>
+      <c r="C32" s="0" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
added functional album search and collection view compatible with frontend.
</commit_message>
<xml_diff>
--- a/Database Grading Criteria (2).xlsx
+++ b/Database Grading Criteria (2).xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="50">
   <si>
     <t xml:space="preserve">Grading Element</t>
   </si>
@@ -578,8 +578,8 @@
   </sheetPr>
   <dimension ref="A1:C48"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C33" activeCellId="0" sqref="C33"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B49" activeCellId="0" sqref="B49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.57421875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -702,7 +702,7 @@
       <c r="B11" s="4" t="n">
         <v>2</v>
       </c>
-      <c r="C11" s="0" t="s">
+      <c r="C11" s="1" t="s">
         <v>3</v>
       </c>
     </row>
@@ -713,7 +713,7 @@
       <c r="B12" s="4" t="n">
         <v>4</v>
       </c>
-      <c r="C12" s="0" t="s">
+      <c r="C12" s="1" t="s">
         <v>3</v>
       </c>
     </row>
@@ -821,7 +821,7 @@
       <c r="B22" s="4" t="n">
         <v>2</v>
       </c>
-      <c r="C22" s="0" t="s">
+      <c r="C22" s="1" t="s">
         <v>3</v>
       </c>
     </row>
@@ -899,7 +899,9 @@
       <c r="B30" s="4" t="n">
         <v>1</v>
       </c>
-      <c r="C30" s="1"/>
+      <c r="C30" s="1" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="6" t="s">
@@ -908,7 +910,9 @@
       <c r="B31" s="4" t="n">
         <v>1</v>
       </c>
-      <c r="C31" s="1"/>
+      <c r="C31" s="1" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="6" t="s">
@@ -917,7 +921,7 @@
       <c r="B32" s="4" t="n">
         <v>2</v>
       </c>
-      <c r="C32" s="0" t="s">
+      <c r="C32" s="1" t="s">
         <v>3</v>
       </c>
     </row>
@@ -936,6 +940,9 @@
       <c r="B34" s="4" t="n">
         <v>2</v>
       </c>
+      <c r="C34" s="0" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="6" t="s">
@@ -944,6 +951,9 @@
       <c r="B35" s="4" t="n">
         <v>1</v>
       </c>
+      <c r="C35" s="0" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="6" t="s">
@@ -1025,6 +1035,9 @@
       </c>
       <c r="B45" s="4" t="n">
         <v>2</v>
+      </c>
+      <c r="C45" s="0" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>